<commit_message>
add test part 1
</commit_message>
<xml_diff>
--- a/reports/Sales-MARCH.xlsx
+++ b/reports/Sales-MARCH.xlsx
@@ -35,16 +35,16 @@
     <t>Walter White</t>
   </si>
   <si>
+    <t>GOTW771012HMRGR087</t>
+  </si>
+  <si>
+    <t>Khal Drogo</t>
+  </si>
+  <si>
     <t>WALA771012HCRGR054</t>
   </si>
   <si>
     <t>Wednesday Addams</t>
-  </si>
-  <si>
-    <t>GOTW771012HMRGR087</t>
-  </si>
-  <si>
-    <t>Khal Drogo</t>
   </si>
 </sst>
 </file>
@@ -171,7 +171,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n" s="2">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>